<commit_message>
tablas precisión y subida1
</commit_message>
<xml_diff>
--- a/Datos cultivos productivos/Fases producción v02.xlsx
+++ b/Datos cultivos productivos/Fases producción v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Datathon 24\Datos cultivos productivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\Datathon\Data\Datathon-24\Datos cultivos productivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8346EF22-D5FB-41B4-BD94-BB261E20FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F846C4-56DB-4F2D-9AFE-2E8AD125CB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F23BFB18-183F-4DC7-8A7A-CA1EEB347B74}"/>
+    <workbookView xWindow="38280" yWindow="3510" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{F23BFB18-183F-4DC7-8A7A-CA1EEB347B74}"/>
   </bookViews>
   <sheets>
     <sheet name="Preinóculo" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="30">
   <si>
     <t>pH</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>1,82+e08</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -1704,26 +1707,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8912624-0F58-4DA9-A671-5761765520A7}">
   <dimension ref="A1:U168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="8"/>
-    <col min="6" max="6" width="11.44140625" style="21"/>
-    <col min="7" max="8" width="11.44140625" style="8"/>
-    <col min="9" max="9" width="11.44140625" style="21"/>
-    <col min="10" max="13" width="11.44140625" style="8"/>
-    <col min="14" max="21" width="10.44140625"/>
+    <col min="3" max="3" width="27.42578125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="8"/>
+    <col min="6" max="6" width="11.42578125" style="21"/>
+    <col min="7" max="8" width="11.42578125" style="8"/>
+    <col min="9" max="9" width="11.42578125" style="21"/>
+    <col min="10" max="13" width="11.42578125" style="8"/>
+    <col min="14" max="21" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="51"/>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -1745,7 +1748,7 @@
       <c r="M1"/>
       <c r="N1"/>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>3</v>
       </c>
@@ -1792,7 +1795,7 @@
       <c r="T2"/>
       <c r="U2"/>
     </row>
-    <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="30">
         <v>23023</v>
       </c>
@@ -1830,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>23024</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>23025</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>23026</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>23027</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
         <v>23028</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>23029</v>
       </c>
@@ -2058,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>23030</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>23031</v>
       </c>
@@ -2134,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>23032</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>23033</v>
       </c>
@@ -2210,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>23034</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>23035</v>
       </c>
@@ -2286,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>23036</v>
       </c>
@@ -2324,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>23037</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>23038</v>
       </c>
@@ -2400,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>23039</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>23040</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <v>23041</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>23042</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <v>23044</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
         <v>23043</v>
       </c>
@@ -2628,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="24">
         <v>23045</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24">
         <v>23046</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
         <v>23047</v>
       </c>
@@ -2742,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
         <v>23048</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <v>23049</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="24">
         <v>23050</v>
       </c>
@@ -2856,7 +2859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>23051</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24">
         <v>23052</v>
       </c>
@@ -2932,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>23053</v>
       </c>
@@ -2970,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24">
         <v>23054</v>
       </c>
@@ -3008,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <v>23055</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24">
         <v>23056</v>
       </c>
@@ -3084,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24">
         <v>23957</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="24">
         <v>23060</v>
       </c>
@@ -3160,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24">
         <v>23061</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24">
         <v>23062</v>
       </c>
@@ -3236,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24">
         <v>23063</v>
       </c>
@@ -3274,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24">
         <v>23064</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
         <v>23065</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25">
         <v>23067</v>
       </c>
@@ -3388,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="24">
         <v>23068</v>
       </c>
@@ -3426,7 +3429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25">
         <v>23069</v>
       </c>
@@ -3464,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="24">
         <v>23066</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24">
         <v>23070</v>
       </c>
@@ -3540,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24">
         <v>23071</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25">
         <v>23072</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="24">
         <v>23073</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25">
         <v>23075</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="24">
         <v>23074</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24">
         <v>23076</v>
       </c>
@@ -3768,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="24">
         <v>23077</v>
       </c>
@@ -3806,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <v>23078</v>
       </c>
@@ -3844,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="24">
         <v>23079</v>
       </c>
@@ -3882,7 +3885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <v>23080</v>
       </c>
@@ -3920,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="24">
         <v>23081</v>
       </c>
@@ -3958,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24">
         <v>23082</v>
       </c>
@@ -3996,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="24">
         <v>23083</v>
       </c>
@@ -4034,7 +4037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="25">
         <v>23084</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="24">
         <v>23085</v>
       </c>
@@ -4110,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25">
         <v>23086</v>
       </c>
@@ -4148,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="24">
         <v>23087</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="25">
         <v>23088</v>
       </c>
@@ -4224,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="29">
         <v>23089</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="24">
         <v>23090</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="24">
         <v>23091</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="24">
         <v>23092</v>
       </c>
@@ -4376,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24">
         <v>23094</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24">
         <v>23095</v>
       </c>
@@ -4452,7 +4455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24">
         <v>23096</v>
       </c>
@@ -4490,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24">
         <v>23097</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24">
         <v>23098</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24">
         <v>23099</v>
       </c>
@@ -4604,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24">
         <v>23100</v>
       </c>
@@ -4642,7 +4645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24">
         <v>23101</v>
       </c>
@@ -4680,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="25">
         <v>23102</v>
       </c>
@@ -4718,7 +4721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="24">
         <v>23103</v>
       </c>
@@ -4756,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24">
         <v>23104</v>
       </c>
@@ -4794,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="24">
         <v>23105</v>
       </c>
@@ -4832,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24">
         <v>23108</v>
       </c>
@@ -4870,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="24">
         <v>23109</v>
       </c>
@@ -4908,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="24">
         <v>23110</v>
       </c>
@@ -4946,7 +4949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="25">
         <v>23111</v>
       </c>
@@ -4984,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="24">
         <v>23112</v>
       </c>
@@ -5022,7 +5025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="24">
         <v>23113</v>
       </c>
@@ -5060,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="24" t="s">
         <v>11</v>
       </c>
@@ -5098,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="24">
         <v>23114</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="24">
         <v>23117</v>
       </c>
@@ -5174,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24">
         <v>23118</v>
       </c>
@@ -5212,7 +5215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="24">
         <v>23119</v>
       </c>
@@ -5250,7 +5253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="24">
         <v>23120</v>
       </c>
@@ -5288,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="25">
         <v>23121</v>
       </c>
@@ -5326,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="24">
         <v>23124</v>
       </c>
@@ -5364,7 +5367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="24">
         <v>23125</v>
       </c>
@@ -5402,7 +5405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="24">
         <v>23126</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="24">
         <v>23127</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="24">
         <v>23131</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="24">
         <v>23132</v>
       </c>
@@ -5554,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="25">
         <v>23133</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="24">
         <v>23136</v>
       </c>
@@ -5630,7 +5633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="24">
         <v>23137</v>
       </c>
@@ -5668,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="24">
         <v>23138</v>
       </c>
@@ -5706,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="24">
         <v>23139</v>
       </c>
@@ -5744,7 +5747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="24">
         <v>24004</v>
       </c>
@@ -5782,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="24">
         <v>24002</v>
       </c>
@@ -5820,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="24">
         <v>24003</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="25">
         <v>24005</v>
       </c>
@@ -5896,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="24">
         <v>24007</v>
       </c>
@@ -5934,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="24">
         <v>24008</v>
       </c>
@@ -5972,7 +5975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="24">
         <v>24009</v>
       </c>
@@ -6010,7 +6013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="24">
         <v>24010</v>
       </c>
@@ -6048,7 +6051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="24">
         <v>24012</v>
       </c>
@@ -6086,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="24">
         <v>24020</v>
       </c>
@@ -6124,7 +6127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="24">
         <v>24019</v>
       </c>
@@ -6162,7 +6165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="24">
         <v>24020</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="24">
         <v>24021</v>
       </c>
@@ -6238,7 +6241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="24">
         <v>24014</v>
       </c>
@@ -6276,7 +6279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="25">
         <v>24027</v>
       </c>
@@ -6314,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="24">
         <v>24031</v>
       </c>
@@ -6352,7 +6355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="24">
         <v>24035</v>
       </c>
@@ -6390,7 +6393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="24">
         <v>24036</v>
       </c>
@@ -6428,7 +6431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="24">
         <v>24041</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="24">
         <v>24042</v>
       </c>
@@ -6504,7 +6507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="24">
         <v>24043</v>
       </c>
@@ -6542,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="25">
         <v>24045</v>
       </c>
@@ -6580,7 +6583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="25">
         <v>24044</v>
       </c>
@@ -6618,7 +6621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="25">
         <v>24049</v>
       </c>
@@ -6656,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="24">
         <v>24050</v>
       </c>
@@ -6694,7 +6697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="24">
         <v>24051</v>
       </c>
@@ -6732,7 +6735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="24">
         <v>24055</v>
       </c>
@@ -6770,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="24">
         <v>24056</v>
       </c>
@@ -6808,7 +6811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="24">
         <v>24054</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="24">
         <v>24057</v>
       </c>
@@ -6884,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="24">
         <v>24060</v>
       </c>
@@ -6922,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="24">
         <v>24061</v>
       </c>
@@ -6960,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="24">
         <v>24063</v>
       </c>
@@ -6998,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="24">
         <v>24064</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="24">
         <v>24067</v>
       </c>
@@ -7074,7 +7077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="24">
         <v>24070</v>
       </c>
@@ -7112,7 +7115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="24">
         <v>24071</v>
       </c>
@@ -7150,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="24">
         <v>24072</v>
       </c>
@@ -7188,7 +7191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="24">
         <v>24073</v>
       </c>
@@ -7226,7 +7229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="24">
         <v>24074</v>
       </c>
@@ -7264,7 +7267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="24">
         <v>24075</v>
       </c>
@@ -7302,7 +7305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="24">
         <v>24076</v>
       </c>
@@ -7340,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="24">
         <v>24077</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="24">
         <v>24078</v>
       </c>
@@ -7416,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="24">
         <v>24081</v>
       </c>
@@ -7454,7 +7457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="24">
         <v>24083</v>
       </c>
@@ -7492,7 +7495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="24">
         <v>24084</v>
       </c>
@@ -7530,7 +7533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="24">
         <v>24085</v>
       </c>
@@ -7568,7 +7571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="24">
         <v>24088</v>
       </c>
@@ -7606,7 +7609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="24">
         <v>24089</v>
       </c>
@@ -7644,7 +7647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="24">
         <v>24091</v>
       </c>
@@ -7682,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="24">
         <v>24092</v>
       </c>
@@ -7720,7 +7723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="24">
         <v>24095</v>
       </c>
@@ -7758,7 +7761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="24">
         <v>24097</v>
       </c>
@@ -7796,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="24">
         <v>24098</v>
       </c>
@@ -7834,7 +7837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="24">
         <v>24101</v>
       </c>
@@ -7872,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="24">
         <v>24103</v>
       </c>
@@ -7910,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="24">
         <v>24104</v>
       </c>
@@ -7948,7 +7951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="24">
         <v>24105</v>
       </c>
@@ -7986,7 +7989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="24">
         <v>24108</v>
       </c>
@@ -8024,7 +8027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="24">
         <v>24111</v>
       </c>
@@ -8062,7 +8065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="24"/>
       <c r="B168" s="27"/>
       <c r="C168" s="45"/>
@@ -8099,19 +8102,19 @@
       <selection pane="bottomRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="46" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="46" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="36"/>
-    <col min="7" max="7" width="11.44140625" style="3"/>
-    <col min="8" max="8" width="14.88671875" style="43" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="36" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="46" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="46" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="36"/>
+    <col min="7" max="7" width="11.42578125" style="3"/>
+    <col min="8" max="8" width="14.85546875" style="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>3</v>
       </c>
@@ -8137,7 +8140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>23019</v>
       </c>
@@ -8163,7 +8166,7 @@
         <v>134400000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>23020</v>
       </c>
@@ -8190,7 +8193,7 @@
       </c>
       <c r="J3" s="63"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>23021</v>
       </c>
@@ -8216,7 +8219,7 @@
         <v>115200000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>23022</v>
       </c>
@@ -8242,7 +8245,7 @@
         <v>115200000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>23023</v>
       </c>
@@ -8268,7 +8271,7 @@
         <v>106400000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>23024</v>
       </c>
@@ -8294,7 +8297,7 @@
         <v>106400000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="37">
         <v>23025</v>
       </c>
@@ -8320,7 +8323,7 @@
         <v>84800000</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>23026</v>
       </c>
@@ -8346,7 +8349,7 @@
         <v>84800000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="37">
         <v>23027</v>
       </c>
@@ -8372,7 +8375,7 @@
         <v>104800000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>23028</v>
       </c>
@@ -8398,7 +8401,7 @@
         <v>104800000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="37">
         <v>23029</v>
       </c>
@@ -8424,7 +8427,7 @@
         <v>96800000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="37">
         <v>23030</v>
       </c>
@@ -8450,7 +8453,7 @@
         <v>96800000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
         <v>23031</v>
       </c>
@@ -8476,7 +8479,7 @@
         <v>105600000</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>23032</v>
       </c>
@@ -8502,7 +8505,7 @@
         <v>105600000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="37">
         <v>23033</v>
       </c>
@@ -8528,7 +8531,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="37">
         <v>23034</v>
       </c>
@@ -8554,7 +8557,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="37">
         <v>23035</v>
       </c>
@@ -8580,7 +8583,7 @@
         <v>81600000</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
         <v>23036</v>
       </c>
@@ -8606,7 +8609,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="37">
         <v>23037</v>
       </c>
@@ -8632,7 +8635,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="37">
         <v>23038</v>
       </c>
@@ -8658,7 +8661,7 @@
         <v>115200000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="37">
         <v>23039</v>
       </c>
@@ -8684,7 +8687,7 @@
         <v>115200000</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37">
         <v>23040</v>
       </c>
@@ -8710,7 +8713,7 @@
         <v>154400000</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="37">
         <v>23041</v>
       </c>
@@ -8736,7 +8739,7 @@
         <v>107200000</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
         <v>23042</v>
       </c>
@@ -8762,7 +8765,7 @@
         <v>108800000</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="37">
         <v>23044</v>
       </c>
@@ -8788,7 +8791,7 @@
         <v>75767200</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="37">
         <v>23043</v>
       </c>
@@ -8814,7 +8817,7 @@
         <v>87200000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="37">
         <v>23045</v>
       </c>
@@ -8840,7 +8843,7 @@
         <v>87200000</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="37">
         <v>23046</v>
       </c>
@@ -8866,7 +8869,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="37">
         <v>23047</v>
       </c>
@@ -8892,7 +8895,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37">
         <v>23048</v>
       </c>
@@ -8918,7 +8921,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="37">
         <v>23049</v>
       </c>
@@ -8944,7 +8947,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="37">
         <v>23050</v>
       </c>
@@ -8970,7 +8973,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="37">
         <v>23051</v>
       </c>
@@ -8996,7 +8999,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="37">
         <v>23052</v>
       </c>
@@ -9022,7 +9025,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="37">
         <v>23053</v>
       </c>
@@ -9048,7 +9051,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="37">
         <v>23054</v>
       </c>
@@ -9074,7 +9077,7 @@
         <v>85600000</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="38">
         <v>23055</v>
       </c>
@@ -9100,7 +9103,7 @@
         <v>85600000</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="37">
         <v>23056</v>
       </c>
@@ -9126,7 +9129,7 @@
         <v>112000000</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="37">
         <v>23057</v>
       </c>
@@ -9152,7 +9155,7 @@
         <v>112000000</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="37">
         <v>23060</v>
       </c>
@@ -9178,7 +9181,7 @@
         <v>103200000</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
         <v>23061</v>
       </c>
@@ -9204,7 +9207,7 @@
         <v>103200000</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="37">
         <v>23062</v>
       </c>
@@ -9230,7 +9233,7 @@
         <v>101600000</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="37">
         <v>23063</v>
       </c>
@@ -9256,7 +9259,7 @@
         <v>101600000</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="37">
         <v>23064</v>
       </c>
@@ -9282,7 +9285,7 @@
         <v>112000000</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="38">
         <v>23065</v>
       </c>
@@ -9308,7 +9311,7 @@
         <v>112000000</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="38">
         <v>23067</v>
       </c>
@@ -9334,7 +9337,7 @@
         <v>130400000</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="37">
         <v>23068</v>
       </c>
@@ -9360,7 +9363,7 @@
         <v>131200000</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="37">
         <v>23069</v>
       </c>
@@ -9386,7 +9389,7 @@
         <v>131200000</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="37">
         <v>23066</v>
       </c>
@@ -9412,7 +9415,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="37">
         <v>23070</v>
       </c>
@@ -9438,7 +9441,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="37">
         <v>23071</v>
       </c>
@@ -9464,7 +9467,7 @@
         <v>76800000</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="38">
         <v>23072</v>
       </c>
@@ -9490,7 +9493,7 @@
         <v>76800000</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="37">
         <v>23073</v>
       </c>
@@ -9516,7 +9519,7 @@
         <v>111200000</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="37">
         <v>23074</v>
       </c>
@@ -9542,7 +9545,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="37">
         <v>23075</v>
       </c>
@@ -9568,7 +9571,7 @@
         <v>111200000</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="38">
         <v>23076</v>
       </c>
@@ -9594,7 +9597,7 @@
         <v>92000000</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37">
         <v>23077</v>
       </c>
@@ -9620,7 +9623,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="37">
         <v>23078</v>
       </c>
@@ -9646,7 +9649,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="37">
         <v>23079</v>
       </c>
@@ -9672,7 +9675,7 @@
         <v>92800000</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="37">
         <v>23080</v>
       </c>
@@ -9698,7 +9701,7 @@
         <v>92800000</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="37">
         <v>23081</v>
       </c>
@@ -9724,7 +9727,7 @@
         <v>79840000</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="37">
         <v>23082</v>
       </c>
@@ -9750,7 +9753,7 @@
         <v>79840000</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="37">
         <v>23083</v>
       </c>
@@ -9776,7 +9779,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="38">
         <v>23084</v>
       </c>
@@ -9802,7 +9805,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="37">
         <v>23085</v>
       </c>
@@ -9828,7 +9831,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="37">
         <v>23086</v>
       </c>
@@ -9854,7 +9857,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="37">
         <v>23087</v>
       </c>
@@ -9880,7 +9883,7 @@
         <v>82480000</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="38">
         <v>23088</v>
       </c>
@@ -9906,7 +9909,7 @@
         <v>82480000</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>23089</v>
       </c>
@@ -9932,7 +9935,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="41">
         <v>23090</v>
       </c>
@@ -9958,7 +9961,7 @@
         <v>86400000</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="22">
         <v>23091</v>
       </c>
@@ -9984,7 +9987,7 @@
         <v>96000000</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="22">
         <v>23092</v>
       </c>
@@ -10010,7 +10013,7 @@
         <v>96000000</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="37">
         <v>23094</v>
       </c>
@@ -10036,7 +10039,7 @@
         <v>94400000</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="37">
         <v>23095</v>
       </c>
@@ -10062,7 +10065,7 @@
         <v>94400000</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="37">
         <v>23096</v>
       </c>
@@ -10088,7 +10091,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="37">
         <v>23097</v>
       </c>
@@ -10114,7 +10117,7 @@
         <v>89600000</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="37">
         <v>23098</v>
       </c>
@@ -10141,7 +10144,7 @@
       </c>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="37">
         <v>23099</v>
       </c>
@@ -10168,7 +10171,7 @@
       </c>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="37">
         <v>23100</v>
       </c>
@@ -10194,7 +10197,7 @@
         <v>81600000</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="37">
         <v>23101</v>
       </c>
@@ -10220,7 +10223,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="38">
         <v>23102</v>
       </c>
@@ -10246,7 +10249,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="37">
         <v>23103</v>
       </c>
@@ -10272,7 +10275,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="37">
         <v>23104</v>
       </c>
@@ -10298,7 +10301,7 @@
         <v>90400000</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="37">
         <v>23105</v>
       </c>
@@ -10324,7 +10327,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="37">
         <v>23108</v>
       </c>
@@ -10350,7 +10353,7 @@
         <v>99200000</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="37">
         <v>23109</v>
       </c>
@@ -10376,7 +10379,7 @@
         <v>99200000</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="37">
         <v>23110</v>
       </c>
@@ -10402,7 +10405,7 @@
         <v>84000000</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="38">
         <v>23111</v>
       </c>
@@ -10428,7 +10431,7 @@
         <v>84000000</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="37">
         <v>23112</v>
       </c>
@@ -10454,7 +10457,7 @@
         <v>97600000</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="37">
         <v>23113</v>
       </c>
@@ -10480,7 +10483,7 @@
         <v>97600000</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="37" t="s">
         <v>11</v>
       </c>
@@ -10506,7 +10509,7 @@
         <v>142400000</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="37">
         <v>23114</v>
       </c>
@@ -10532,7 +10535,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="37">
         <v>23117</v>
       </c>
@@ -10558,7 +10561,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="37">
         <v>23118</v>
       </c>
@@ -10584,7 +10587,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="37">
         <v>23119</v>
       </c>
@@ -10610,7 +10613,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="37">
         <v>23120</v>
       </c>
@@ -10636,7 +10639,7 @@
         <v>104800000</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="37">
         <v>23121</v>
       </c>
@@ -10662,7 +10665,7 @@
         <v>143200000</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="37">
         <v>23124</v>
       </c>
@@ -10688,7 +10691,7 @@
         <v>88800000</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="37">
         <v>23125</v>
       </c>
@@ -10714,7 +10717,7 @@
         <v>88800000</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="37">
         <v>23126</v>
       </c>
@@ -10740,7 +10743,7 @@
         <v>134400000</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="38">
         <v>23127</v>
       </c>
@@ -10766,7 +10769,7 @@
         <v>134400000</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="37">
         <v>23131</v>
       </c>
@@ -10792,7 +10795,7 @@
         <v>144800000</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="38">
         <v>23132</v>
       </c>
@@ -10818,7 +10821,7 @@
         <v>101600000</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="37">
         <v>23133</v>
       </c>
@@ -10844,7 +10847,7 @@
         <v>101600000</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="37">
         <v>23136</v>
       </c>
@@ -10870,7 +10873,7 @@
         <v>122400000</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="37">
         <v>23137</v>
       </c>
@@ -10896,7 +10899,7 @@
         <v>167200000</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="37">
         <v>23138</v>
       </c>
@@ -10922,7 +10925,7 @@
         <v>252000000</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="37">
         <v>23139</v>
       </c>
@@ -10948,7 +10951,7 @@
         <v>56800000</v>
       </c>
     </row>
-    <row r="110" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="37">
         <v>24004</v>
       </c>
@@ -10975,7 +10978,7 @@
       </c>
       <c r="K110"/>
     </row>
-    <row r="111" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="37">
         <v>24002</v>
       </c>
@@ -11002,7 +11005,7 @@
       </c>
       <c r="K111"/>
     </row>
-    <row r="112" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="37">
         <v>24003</v>
       </c>
@@ -11029,7 +11032,7 @@
       </c>
       <c r="K112"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="37">
         <v>24005</v>
       </c>
@@ -11055,7 +11058,7 @@
         <v>79760000</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="37">
         <v>24007</v>
       </c>
@@ -11081,7 +11084,7 @@
         <v>79440000</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="37">
         <v>24008</v>
       </c>
@@ -11107,7 +11110,7 @@
         <v>79440000</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="37">
         <v>24009</v>
       </c>
@@ -11133,7 +11136,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="37">
         <v>24010</v>
       </c>
@@ -11159,7 +11162,7 @@
         <v>95200000</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="37">
         <v>24012</v>
       </c>
@@ -11185,7 +11188,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="37">
         <v>24020</v>
       </c>
@@ -11211,7 +11214,7 @@
         <v>95200000</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="37">
         <v>24019</v>
       </c>
@@ -11237,7 +11240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="37">
         <v>24020</v>
       </c>
@@ -11263,7 +11266,7 @@
         <v>95200000</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="38">
         <v>24021</v>
       </c>
@@ -11289,7 +11292,7 @@
         <v>101600000</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="37">
         <v>24014</v>
       </c>
@@ -11315,7 +11318,7 @@
         <v>37040000</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="38">
         <v>24027</v>
       </c>
@@ -11341,7 +11344,7 @@
         <v>37040000</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="38">
         <v>24031</v>
       </c>
@@ -11367,7 +11370,7 @@
         <v>66640000</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="37">
         <v>24035</v>
       </c>
@@ -11393,7 +11396,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="37">
         <v>24036</v>
       </c>
@@ -11419,7 +11422,7 @@
         <v>88000000</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="37">
         <v>24041</v>
       </c>
@@ -11445,7 +11448,7 @@
         <v>134400000</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="37">
         <v>24042</v>
       </c>
@@ -11471,7 +11474,7 @@
         <v>134400000</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="38">
         <v>24043</v>
       </c>
@@ -11497,7 +11500,7 @@
         <v>109600000</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="37">
         <v>24045</v>
       </c>
@@ -11523,7 +11526,7 @@
         <v>109600000</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="38">
         <v>24044</v>
       </c>
@@ -11549,7 +11552,7 @@
         <v>104800000</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="38">
         <v>24049</v>
       </c>
@@ -11575,7 +11578,7 @@
         <v>104800000</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="38">
         <v>24050</v>
       </c>
@@ -11601,7 +11604,7 @@
         <v>102400000</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="38">
         <v>24051</v>
       </c>
@@ -11627,7 +11630,7 @@
         <v>102400000</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="24">
         <v>24055</v>
       </c>
@@ -11653,7 +11656,7 @@
         <v>159200000</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="24">
         <v>24056</v>
       </c>
@@ -11679,7 +11682,7 @@
         <v>159200000</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="24">
         <v>24054</v>
       </c>
@@ -11705,7 +11708,7 @@
         <v>121600000</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="24">
         <v>24057</v>
       </c>
@@ -11731,7 +11734,7 @@
         <v>121600000</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="24">
         <v>24060</v>
       </c>
@@ -11758,7 +11761,7 @@
       </c>
       <c r="K140" s="3"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="24">
         <v>24061</v>
       </c>
@@ -11784,7 +11787,7 @@
         <v>125600000</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="24">
         <v>24063</v>
       </c>
@@ -11810,7 +11813,7 @@
         <v>72640000</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="30">
         <v>24064</v>
       </c>
@@ -11836,7 +11839,7 @@
         <v>72640000</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="37">
         <v>24067</v>
       </c>
@@ -11862,7 +11865,7 @@
         <v>120000000</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="37">
         <v>24070</v>
       </c>
@@ -11888,7 +11891,7 @@
         <v>120000000</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="37">
         <v>24071</v>
       </c>
@@ -11914,7 +11917,7 @@
         <v>84000000</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="37">
         <v>24072</v>
       </c>
@@ -11940,7 +11943,7 @@
         <v>144800000</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="37">
         <v>24073</v>
       </c>
@@ -11966,7 +11969,7 @@
         <v>142400000</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="37">
         <v>24074</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>129600000</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="37">
         <v>24075</v>
       </c>
@@ -12018,7 +12021,7 @@
         <v>142400000</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="37">
         <v>24076</v>
       </c>
@@ -12044,7 +12047,7 @@
         <v>129600000</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="37">
         <v>24077</v>
       </c>
@@ -12070,7 +12073,7 @@
         <v>122400000</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="37">
         <v>24078</v>
       </c>
@@ -12096,7 +12099,7 @@
         <v>122400000</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="37">
         <v>24081</v>
       </c>
@@ -12122,7 +12125,7 @@
         <v>122400000</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="37">
         <v>24083</v>
       </c>
@@ -12148,7 +12151,7 @@
         <v>124800000</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="37">
         <v>24084</v>
       </c>
@@ -12174,7 +12177,7 @@
         <v>124800000</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="37">
         <v>24085</v>
       </c>
@@ -12200,7 +12203,7 @@
         <v>122400000</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="37">
         <v>24088</v>
       </c>
@@ -12226,7 +12229,7 @@
         <v>129600000</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="37">
         <v>24089</v>
       </c>
@@ -12252,7 +12255,7 @@
         <v>129600000</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="37">
         <v>24091</v>
       </c>
@@ -12278,7 +12281,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="37">
         <v>24092</v>
       </c>
@@ -12304,7 +12307,7 @@
         <v>104000000</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="37">
         <v>24095</v>
       </c>
@@ -12330,7 +12333,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="37">
         <v>24097</v>
       </c>
@@ -12356,7 +12359,7 @@
         <v>83200000</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="37">
         <v>24098</v>
       </c>
@@ -12382,7 +12385,7 @@
         <v>54240000</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="37">
         <v>24101</v>
       </c>
@@ -12408,7 +12411,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="37">
         <v>24103</v>
       </c>
@@ -12434,7 +12437,7 @@
         <v>91200000</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="37">
         <v>24104</v>
       </c>
@@ -12460,7 +12463,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="37">
         <v>24105</v>
       </c>
@@ -12486,7 +12489,7 @@
         <v>82400000</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="37">
         <v>24108</v>
       </c>
@@ -12512,7 +12515,7 @@
         <v>92800000</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="37"/>
       <c r="B170" s="37"/>
       <c r="C170" s="47"/>
@@ -12522,7 +12525,7 @@
       <c r="G170" s="14"/>
       <c r="H170" s="44"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="37"/>
       <c r="B171" s="37"/>
       <c r="C171" s="47"/>
@@ -12544,34 +12547,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57038628-FF83-407A-834B-B9AC80743F74}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q133" sqref="Q133"/>
+      <selection pane="bottomRight" activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="6"/>
-    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="6"/>
+    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="6" customWidth="1"/>
     <col min="13" max="13" width="16" style="6" customWidth="1"/>
-    <col min="14" max="15" width="9.88671875" style="6" customWidth="1"/>
+    <col min="14" max="15" width="9.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>3</v>
       </c>
@@ -12618,7 +12622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="102">
         <v>23019</v>
       </c>
@@ -12665,7 +12669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="102">
         <v>23020</v>
       </c>
@@ -12712,7 +12716,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="102">
         <v>23021</v>
       </c>
@@ -12761,7 +12765,7 @@
       <c r="P4" s="63"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="103">
         <v>23022</v>
       </c>
@@ -12808,7 +12812,7 @@
         <v>5.9200000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="103">
         <v>23023</v>
       </c>
@@ -12855,7 +12859,7 @@
         <v>2.9600000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="103">
         <v>23024</v>
       </c>
@@ -12902,7 +12906,7 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="103">
         <v>23025</v>
       </c>
@@ -12949,7 +12953,7 @@
         <v>4.4799999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="103">
         <v>23026</v>
       </c>
@@ -12996,7 +13000,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="103">
         <v>23027</v>
       </c>
@@ -13044,7 +13048,7 @@
       </c>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="103">
         <v>23028</v>
       </c>
@@ -13091,7 +13095,7 @@
         <v>4.7200000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="103">
         <v>23029</v>
       </c>
@@ -13138,7 +13142,7 @@
         <v>6.7200000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="103">
         <v>23030</v>
       </c>
@@ -13185,7 +13189,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="103">
         <v>23031</v>
       </c>
@@ -13232,7 +13236,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="103">
         <v>23032</v>
       </c>
@@ -13279,7 +13283,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="103">
         <v>23033</v>
       </c>
@@ -13326,7 +13330,7 @@
         <v>5.5200000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="103">
         <v>23034</v>
       </c>
@@ -13373,7 +13377,7 @@
         <v>5.5200000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="103">
         <v>23035</v>
       </c>
@@ -13420,7 +13424,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="103">
         <v>23036</v>
       </c>
@@ -13467,7 +13471,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="103">
         <v>23038</v>
       </c>
@@ -13514,7 +13518,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="103">
         <v>23039</v>
       </c>
@@ -13561,7 +13565,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="103">
         <v>23040</v>
       </c>
@@ -13608,7 +13612,7 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="103">
         <v>23041</v>
       </c>
@@ -13655,7 +13659,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="103">
         <v>23042</v>
       </c>
@@ -13702,7 +13706,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="103">
         <v>23044</v>
       </c>
@@ -13749,7 +13753,7 @@
         <v>4.9600000000000009</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="103">
         <v>23043</v>
       </c>
@@ -13796,7 +13800,7 @@
         <v>4.4799999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="103">
         <v>23045</v>
       </c>
@@ -13843,7 +13847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="103">
         <v>23046</v>
       </c>
@@ -13890,7 +13894,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="103">
         <v>23047</v>
       </c>
@@ -13937,7 +13941,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="103">
         <v>23048</v>
       </c>
@@ -13984,7 +13988,7 @@
         <v>5.6000000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="103">
         <v>23049</v>
       </c>
@@ -14031,7 +14035,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="103">
         <v>23050</v>
       </c>
@@ -14079,7 +14083,7 @@
       </c>
       <c r="R32" s="3"/>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="103">
         <v>23051</v>
       </c>
@@ -14126,7 +14130,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="103">
         <v>23053</v>
       </c>
@@ -14173,7 +14177,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="103">
         <v>23054</v>
       </c>
@@ -14220,7 +14224,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="103">
         <v>23055</v>
       </c>
@@ -14267,7 +14271,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="103">
         <v>23056</v>
       </c>
@@ -14314,7 +14318,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="103">
         <v>23057</v>
       </c>
@@ -14361,7 +14365,7 @@
         <v>5.9200000000000008</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="103">
         <v>23060</v>
       </c>
@@ -14408,7 +14412,7 @@
         <v>7.120000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="103">
         <v>23061</v>
       </c>
@@ -14455,7 +14459,7 @@
         <v>7.28</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="103">
         <v>23063</v>
       </c>
@@ -14502,7 +14506,7 @@
         <v>5.9200000000000008</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="103">
         <v>23064</v>
       </c>
@@ -14549,7 +14553,7 @@
         <v>7.4400000000000013</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="103">
         <v>23065</v>
       </c>
@@ -14596,7 +14600,7 @@
         <v>6.6400000000000006</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="103">
         <v>23067</v>
       </c>
@@ -14643,7 +14647,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="103">
         <v>23068</v>
       </c>
@@ -14690,7 +14694,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="103">
         <v>23069</v>
       </c>
@@ -14737,7 +14741,7 @@
         <v>5.6000000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="103">
         <v>23070</v>
       </c>
@@ -14784,7 +14788,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="103">
         <v>23071</v>
       </c>
@@ -14831,7 +14835,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="103">
         <v>23072</v>
       </c>
@@ -14878,7 +14882,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="103">
         <v>23073</v>
       </c>
@@ -14925,7 +14929,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="103">
         <v>23075</v>
       </c>
@@ -14972,7 +14976,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="103">
         <v>23076</v>
       </c>
@@ -15019,7 +15023,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="103">
         <v>23077</v>
       </c>
@@ -15067,7 +15071,7 @@
       </c>
       <c r="R53" s="3"/>
     </row>
-    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="103">
         <v>23078</v>
       </c>
@@ -15114,7 +15118,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="103">
         <v>23079</v>
       </c>
@@ -15161,7 +15165,7 @@
         <v>7.120000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="103">
         <v>23080</v>
       </c>
@@ -15208,7 +15212,7 @@
         <v>7.8400000000000007</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="103">
         <v>23081</v>
       </c>
@@ -15255,7 +15259,7 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="103">
         <v>23082</v>
       </c>
@@ -15302,7 +15306,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="103">
         <v>23083</v>
       </c>
@@ -15349,7 +15353,7 @@
         <v>5.5200000000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="103">
         <v>23084</v>
       </c>
@@ -15396,7 +15400,7 @@
         <v>7.8400000000000007</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="103">
         <v>23085</v>
       </c>
@@ -15443,7 +15447,7 @@
         <v>4.4799999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="103">
         <v>23086</v>
       </c>
@@ -15490,7 +15494,7 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="103">
         <v>23087</v>
       </c>
@@ -15537,7 +15541,7 @@
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="103">
         <v>23088</v>
       </c>
@@ -15584,7 +15588,7 @@
         <v>6.08</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="103">
         <v>23089</v>
       </c>
@@ -15631,7 +15635,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="106">
         <v>23090</v>
       </c>
@@ -15678,7 +15682,7 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="107">
         <v>23091</v>
       </c>
@@ -15725,7 +15729,7 @@
         <v>5.5200000000000005</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="107">
         <v>23092</v>
       </c>
@@ -15772,7 +15776,7 @@
         <v>8.24</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="108">
         <v>23093</v>
       </c>
@@ -15819,7 +15823,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="108">
         <v>23094</v>
       </c>
@@ -15866,7 +15870,7 @@
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="109">
         <v>23095</v>
       </c>
@@ -15913,7 +15917,7 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="108">
         <v>23096</v>
       </c>
@@ -15960,7 +15964,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="108">
         <v>23097</v>
       </c>
@@ -16007,7 +16011,7 @@
         <v>5.7600000000000007</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="109">
         <v>23098</v>
       </c>
@@ -16054,7 +16058,7 @@
         <v>7.4400000000000013</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="108">
         <v>23099</v>
       </c>
@@ -16101,7 +16105,7 @@
         <v>5.9200000000000008</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="108">
         <v>23100</v>
       </c>
@@ -16148,7 +16152,7 @@
         <v>4.9600000000000009</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="108">
         <v>23101</v>
       </c>
@@ -16195,7 +16199,7 @@
         <v>7.4400000000000013</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="109">
         <v>23102</v>
       </c>
@@ -16242,7 +16246,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="108">
         <v>23103</v>
       </c>
@@ -16289,7 +16293,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="108">
         <v>23104</v>
       </c>
@@ -16336,7 +16340,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="108">
         <v>23105</v>
       </c>
@@ -16383,7 +16387,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="108">
         <v>23106</v>
       </c>
@@ -16430,7 +16434,7 @@
         <v>6.7200000000000006</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="109">
         <v>23107</v>
       </c>
@@ -16477,7 +16481,7 @@
         <v>7.76</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="108">
         <v>23108</v>
       </c>
@@ -16524,7 +16528,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="108">
         <v>23109</v>
       </c>
@@ -16571,7 +16575,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="108">
         <v>23110</v>
       </c>
@@ -16618,7 +16622,7 @@
         <v>6.7200000000000006</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="109">
         <v>23111</v>
       </c>
@@ -16665,7 +16669,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="108">
         <v>23112</v>
       </c>
@@ -16712,7 +16716,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="108">
         <v>23113</v>
       </c>
@@ -16759,7 +16763,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="108">
         <v>23114</v>
       </c>
@@ -16806,7 +16810,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="108">
         <v>23115</v>
       </c>
@@ -16853,7 +16857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="108">
         <v>23116</v>
       </c>
@@ -16900,7 +16904,7 @@
         <v>7.8288000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="109">
         <v>23117</v>
       </c>
@@ -16947,7 +16951,7 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="108">
         <v>23118</v>
       </c>
@@ -16994,7 +16998,7 @@
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="108">
         <v>23119</v>
       </c>
@@ -17041,7 +17045,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="108">
         <v>23120</v>
       </c>
@@ -17088,7 +17092,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="108">
         <v>23121</v>
       </c>
@@ -17135,7 +17139,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="108">
         <v>23122</v>
       </c>
@@ -17182,7 +17186,7 @@
         <v>8.48</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="109">
         <v>23123</v>
       </c>
@@ -17229,7 +17233,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="108">
         <v>23124</v>
       </c>
@@ -17276,7 +17280,7 @@
         <v>4.4799999999999995</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="109">
         <v>23125</v>
       </c>
@@ -17323,7 +17327,7 @@
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="108">
         <v>23126</v>
       </c>
@@ -17370,7 +17374,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="109">
         <v>23127</v>
       </c>
@@ -17417,7 +17421,7 @@
         <v>7.0400000000000009</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="108">
         <v>23129</v>
       </c>
@@ -17464,7 +17468,7 @@
         <v>6.24</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="109">
         <v>23130</v>
       </c>
@@ -17511,7 +17515,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="108">
         <v>23131</v>
       </c>
@@ -17558,7 +17562,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="108">
         <v>23132</v>
       </c>
@@ -17605,7 +17609,7 @@
         <v>5.7600000000000007</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="109">
         <v>23133</v>
       </c>
@@ -17652,7 +17656,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="108">
         <v>23134</v>
       </c>
@@ -17699,7 +17703,7 @@
         <v>5.7600000000000007</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="109">
         <v>23135</v>
       </c>
@@ -17746,7 +17750,7 @@
         <v>6.7200000000000006</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="109">
         <v>23136</v>
       </c>
@@ -17793,7 +17797,7 @@
         <v>4.9600000000000009</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="108">
         <v>23137</v>
       </c>
@@ -17840,7 +17844,7 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="108">
         <v>23138</v>
       </c>
@@ -17848,7 +17852,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D113" s="81">
         <v>14615</v>
@@ -17887,7 +17891,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="108">
         <v>23139</v>
       </c>
@@ -17895,7 +17899,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D114" s="80">
         <v>14616</v>
@@ -17934,7 +17938,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="115" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="81">
         <v>24004</v>
       </c>
@@ -17942,7 +17946,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D115" s="81">
         <v>14615</v>
@@ -17983,7 +17987,7 @@
       <c r="Q115"/>
       <c r="R115"/>
     </row>
-    <row r="116" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="80">
         <v>24003</v>
       </c>
@@ -17991,7 +17995,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D116" s="81">
         <v>14614</v>
@@ -18032,7 +18036,7 @@
       <c r="Q116"/>
       <c r="R116"/>
     </row>
-    <row r="117" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="108">
         <v>24005</v>
       </c>
@@ -18040,7 +18044,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D117" s="81">
         <v>14616</v>
@@ -18079,7 +18083,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="108">
         <v>24007</v>
       </c>
@@ -18087,7 +18091,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D118" s="81">
         <v>14617</v>
@@ -18126,7 +18130,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="109">
         <v>24008</v>
       </c>
@@ -18134,7 +18138,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D119" s="80">
         <v>14615</v>
@@ -18173,7 +18177,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="108">
         <v>24011</v>
       </c>
@@ -18181,7 +18185,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D120" s="80">
         <v>13189</v>
@@ -18220,7 +18224,7 @@
         <v>6.6400000000000006</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="108">
         <v>24016</v>
       </c>
@@ -18228,7 +18232,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D121" s="80">
         <v>14616</v>
@@ -18267,7 +18271,7 @@
         <v>8.16</v>
       </c>
     </row>
-    <row r="122" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="109">
         <v>24017</v>
       </c>
@@ -18275,7 +18279,7 @@
         <v>2</v>
       </c>
       <c r="C122" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D122" s="80">
         <v>14617</v>
@@ -18314,7 +18318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="108">
         <v>24009</v>
       </c>
@@ -18322,7 +18326,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D123" s="108">
         <v>14614</v>
@@ -18361,7 +18365,7 @@
         <v>7.52</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="109">
         <v>24012</v>
       </c>
@@ -18369,7 +18373,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D124" s="109">
         <v>13170</v>
@@ -18408,7 +18412,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="108">
         <v>24010</v>
       </c>
@@ -18416,7 +18420,7 @@
         <v>1</v>
       </c>
       <c r="C125" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D125" s="108">
         <v>13169</v>
@@ -18455,7 +18459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="109">
         <v>24020</v>
       </c>
@@ -18463,7 +18467,7 @@
         <v>1</v>
       </c>
       <c r="C126" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D126" s="109">
         <v>13170</v>
@@ -18502,7 +18506,7 @@
         <v>7.9200000000000008</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="108">
         <v>24022</v>
       </c>
@@ -18549,7 +18553,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="109">
         <v>24023</v>
       </c>
@@ -18596,7 +18600,7 @@
         <v>8.9599999999999991</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="108">
         <v>24019</v>
       </c>
@@ -18604,7 +18608,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D129" s="108">
         <v>14617</v>
@@ -18643,7 +18647,7 @@
         <v>5.68</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="109">
         <v>24021</v>
       </c>
@@ -18651,7 +18655,7 @@
         <v>1</v>
       </c>
       <c r="C130" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D130" s="109">
         <v>13169</v>
@@ -18690,7 +18694,7 @@
         <v>6.56</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="108">
         <v>24025</v>
       </c>
@@ -18738,7 +18742,7 @@
       </c>
       <c r="P131" s="122"/>
     </row>
-    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="108">
         <v>24014</v>
       </c>
@@ -18746,7 +18750,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D132" s="108">
         <v>14615</v>
@@ -18786,7 +18790,7 @@
       </c>
       <c r="P132" s="122"/>
     </row>
-    <row r="133" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="108">
         <v>24015</v>
       </c>
@@ -18794,7 +18798,7 @@
         <v>3</v>
       </c>
       <c r="C133" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D133" s="108">
         <v>14616</v>
@@ -18834,7 +18838,7 @@
       </c>
       <c r="P133" s="122"/>
     </row>
-    <row r="134" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="109">
         <v>24027</v>
       </c>
@@ -18842,7 +18846,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D134" s="109">
         <v>13170</v>
@@ -18882,7 +18886,7 @@
       </c>
       <c r="P134" s="122"/>
     </row>
-    <row r="135" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="108">
         <v>24028</v>
       </c>
@@ -18930,7 +18934,7 @@
       </c>
       <c r="P135" s="122"/>
     </row>
-    <row r="136" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="109">
         <v>24031</v>
       </c>
@@ -18938,7 +18942,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D136" s="108">
         <v>13169</v>
@@ -18978,7 +18982,7 @@
       </c>
       <c r="P136" s="122"/>
     </row>
-    <row r="137" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="109">
         <v>24037</v>
       </c>
@@ -19026,7 +19030,7 @@
       </c>
       <c r="P137" s="122"/>
     </row>
-    <row r="138" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="109">
         <v>24038</v>
       </c>
@@ -19074,7 +19078,7 @@
       </c>
       <c r="P138" s="122"/>
     </row>
-    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="108">
         <v>24035</v>
       </c>
@@ -19082,7 +19086,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D139" s="107">
         <v>14614</v>
@@ -19122,7 +19126,7 @@
       </c>
       <c r="P139" s="122"/>
     </row>
-    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="109">
         <v>24036</v>
       </c>
@@ -19130,7 +19134,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D140" s="110">
         <v>14617</v>
@@ -19170,7 +19174,7 @@
       </c>
       <c r="P140" s="122"/>
     </row>
-    <row r="141" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="109">
         <v>24040</v>
       </c>
@@ -19218,7 +19222,7 @@
       </c>
       <c r="P141" s="122"/>
     </row>
-    <row r="142" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="108">
         <v>24041</v>
       </c>
@@ -19226,7 +19230,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D142" s="107">
         <v>13169</v>
@@ -19266,7 +19270,7 @@
       </c>
       <c r="P142" s="122"/>
     </row>
-    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="109">
         <v>24042</v>
       </c>
@@ -19274,7 +19278,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="106" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D143" s="110">
         <v>14615</v>
@@ -19314,7 +19318,7 @@
       </c>
       <c r="P143" s="122"/>
     </row>
-    <row r="144" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="108">
         <v>24046</v>
       </c>
@@ -19362,15 +19366,15 @@
       </c>
       <c r="P144" s="122"/>
     </row>
-    <row r="145" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="109">
         <v>24043</v>
       </c>
       <c r="B145" s="108">
         <v>1</v>
       </c>
-      <c r="C145" s="108" t="s">
-        <v>10</v>
+      <c r="C145" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D145" s="108">
         <v>14614</v>
@@ -19410,15 +19414,15 @@
       </c>
       <c r="P145" s="122"/>
     </row>
-    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="109">
         <v>24045</v>
       </c>
       <c r="B146" s="108">
         <v>1</v>
       </c>
-      <c r="C146" s="108" t="s">
-        <v>10</v>
+      <c r="C146" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D146" s="108">
         <v>14616</v>
@@ -19458,15 +19462,15 @@
       </c>
       <c r="P146" s="122"/>
     </row>
-    <row r="147" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="108">
         <v>24044</v>
       </c>
       <c r="B147" s="108">
         <v>1</v>
       </c>
-      <c r="C147" s="108" t="s">
-        <v>10</v>
+      <c r="C147" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D147" s="108">
         <v>13170</v>
@@ -19506,7 +19510,7 @@
       </c>
       <c r="P147" s="122"/>
     </row>
-    <row r="148" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="115">
         <v>24047</v>
       </c>
@@ -19554,15 +19558,15 @@
       </c>
       <c r="P148" s="122"/>
     </row>
-    <row r="149" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="108">
         <v>24049</v>
       </c>
       <c r="B149" s="108">
         <v>1</v>
       </c>
-      <c r="C149" s="108" t="s">
-        <v>10</v>
+      <c r="C149" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D149" s="108">
         <v>14617</v>
@@ -19602,15 +19606,15 @@
       </c>
       <c r="P149" s="122"/>
     </row>
-    <row r="150" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="108">
         <v>24050</v>
       </c>
       <c r="B150" s="108">
         <v>1</v>
       </c>
-      <c r="C150" s="108" t="s">
-        <v>10</v>
+      <c r="C150" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D150" s="108">
         <v>14614</v>
@@ -19650,15 +19654,15 @@
       </c>
       <c r="P150" s="122"/>
     </row>
-    <row r="151" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="109">
         <v>24051</v>
       </c>
       <c r="B151" s="109">
         <v>1</v>
       </c>
-      <c r="C151" s="109" t="s">
-        <v>10</v>
+      <c r="C151" s="106" t="s">
+        <v>29</v>
       </c>
       <c r="D151" s="109">
         <v>13169</v>
@@ -19698,7 +19702,7 @@
       </c>
       <c r="P151" s="122"/>
     </row>
-    <row r="152" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="108">
         <v>24052</v>
       </c>
@@ -19748,7 +19752,7 @@
       <c r="Q152"/>
       <c r="R152"/>
     </row>
-    <row r="153" spans="1:18" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" s="3" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="108">
         <v>24053</v>
       </c>
@@ -19799,7 +19803,13 @@
       <c r="R153"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O153" xr:uid="{8AC3ED98-A4A2-4B11-8E1B-ED316EE28E4B}"/>
+  <autoFilter ref="A1:O153" xr:uid="{8AC3ED98-A4A2-4B11-8E1B-ED316EE28E4B}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="NA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R2:R153">
     <sortCondition ref="R2:R153"/>
   </sortState>

</xml_diff>